<commit_message>
Limpieza de la columna J
</commit_message>
<xml_diff>
--- a/encuesta.xlsx
+++ b/encuesta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8327" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8326" uniqueCount="704">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1513,9 +1513,6 @@
     <t>2004-junio</t>
   </si>
   <si>
-    <t>Mar del plata</t>
-  </si>
-  <si>
     <t>2015-Febrero</t>
   </si>
   <si>
@@ -1615,7 +1612,7 @@
     <t>Su relación con los profesores y compañeros., Problema con la carrera.</t>
   </si>
   <si>
-    <t>BARCELONA - ESPAÑA</t>
+    <t>Otro pais.</t>
   </si>
   <si>
     <t>2010-febrero</t>
@@ -1634,9 +1631,6 @@
   </si>
   <si>
     <t>Su relación con los profesores y compañeros., Problemas económicos., Problemas familiares., Otra.</t>
-  </si>
-  <si>
-    <t>Azul</t>
   </si>
   <si>
     <t>Medicina general., Odontólogo., Psicopedagogía.</t>
@@ -21050,8 +21044,8 @@
       <c r="I277" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="J277" s="1" t="s">
-        <v>499</v>
+      <c r="J277" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="K277" s="1" t="s">
         <v>76</v>
@@ -21144,7 +21138,7 @@
         <v>36</v>
       </c>
       <c r="F280" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G280" s="1" t="s">
         <v>119</v>
@@ -21153,11 +21147,9 @@
         <v>60</v>
       </c>
       <c r="I280" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="J280" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="J280" s="1"/>
       <c r="K280" s="1" t="s">
         <v>85</v>
       </c>
@@ -21354,7 +21346,7 @@
         <v>58</v>
       </c>
       <c r="F286" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G286" s="1" t="s">
         <v>188</v>
@@ -21454,7 +21446,7 @@
         <v>2011.0</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>34</v>
@@ -21478,7 +21470,7 @@
         <v>43</v>
       </c>
       <c r="O288" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P288" s="1" t="s">
         <v>109</v>
@@ -21658,7 +21650,7 @@
         <v>58</v>
       </c>
       <c r="F294" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G294" s="1">
         <v>2015.0</v>
@@ -21685,7 +21677,7 @@
         <v>43</v>
       </c>
       <c r="O294" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P294" s="1" t="s">
         <v>77</v>
@@ -21758,7 +21750,7 @@
         <v>58</v>
       </c>
       <c r="F296" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G296" s="1" t="s">
         <v>188</v>
@@ -21785,7 +21777,7 @@
         <v>43</v>
       </c>
       <c r="O296" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P296" s="1" t="s">
         <v>109</v>
@@ -21850,7 +21842,7 @@
         <v>58</v>
       </c>
       <c r="F297" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G297" s="1">
         <v>3.0</v>
@@ -21942,7 +21934,7 @@
         <v>484</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>90</v>
@@ -22063,7 +22055,7 @@
         <v>43</v>
       </c>
       <c r="P300" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q300" s="1" t="s">
         <v>65</v>
@@ -22133,7 +22125,7 @@
         <v>58</v>
       </c>
       <c r="F302" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G302" s="1">
         <v>2017.0</v>
@@ -22438,10 +22430,10 @@
         <v>58</v>
       </c>
       <c r="F309" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="G309" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="G309" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="H309" s="1" t="s">
         <v>39</v>
@@ -22468,7 +22460,7 @@
         <v>51</v>
       </c>
       <c r="P309" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q309" s="1" t="s">
         <v>65</v>
@@ -22538,16 +22530,16 @@
         <v>58</v>
       </c>
       <c r="F311" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="G311" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="G311" s="1" t="s">
-        <v>517</v>
       </c>
       <c r="H311" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J311" s="1" t="s">
         <v>62</v>
@@ -22633,7 +22625,7 @@
         <v>39</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J312" s="1" t="s">
         <v>62</v>
@@ -22648,7 +22640,7 @@
         <v>0.0</v>
       </c>
       <c r="N312" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O312" s="1" t="s">
         <v>51</v>
@@ -22675,7 +22667,7 @@
         <v>116</v>
       </c>
       <c r="X312" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Y312" s="1" t="s">
         <v>49</v>
@@ -22730,10 +22722,10 @@
         <v>58</v>
       </c>
       <c r="F314" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="G314" s="5" t="s">
         <v>522</v>
-      </c>
-      <c r="G314" s="5" t="s">
-        <v>523</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>39</v>
@@ -22819,16 +22811,16 @@
         <v>58</v>
       </c>
       <c r="F315" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="G315" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="G315" s="5" t="s">
-        <v>525</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I315" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J315" s="1" t="s">
         <v>62</v>
@@ -22963,7 +22955,7 @@
         <v>99</v>
       </c>
       <c r="S318" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="T318" s="1" t="s">
         <v>81</v>
@@ -23051,10 +23043,10 @@
         <v>58</v>
       </c>
       <c r="F323" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="G323" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="G323" s="5" t="s">
-        <v>529</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>34</v>
@@ -23137,19 +23129,19 @@
         <v>36</v>
       </c>
       <c r="F324" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="G324" s="5" t="s">
         <v>530</v>
-      </c>
-      <c r="G324" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I324" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="J324" s="6" t="s">
         <v>532</v>
-      </c>
-      <c r="J324" s="1" t="s">
-        <v>533</v>
       </c>
       <c r="K324" s="1" t="s">
         <v>63</v>
@@ -23245,7 +23237,7 @@
         <v>58</v>
       </c>
       <c r="F327" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G327" s="1" t="s">
         <v>179</v>
@@ -23342,7 +23334,7 @@
         <v>36</v>
       </c>
       <c r="F329" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G329" s="1">
         <v>1990.0</v>
@@ -23439,22 +23431,22 @@
         <v>57</v>
       </c>
       <c r="E331" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="F331" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="F331" s="5" t="s">
+      <c r="G331" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="G331" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="H331" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I331" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="J331" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
+      </c>
+      <c r="J331" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="K331" s="1" t="s">
         <v>85</v>
@@ -23466,13 +23458,13 @@
         <v>1.0</v>
       </c>
       <c r="N331" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="O331" s="1" t="s">
         <v>44</v>
       </c>
       <c r="P331" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="Q331" s="1" t="s">
         <v>65</v>
@@ -23599,7 +23591,7 @@
         <v>60</v>
       </c>
       <c r="I339" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J339" s="1" t="s">
         <v>62</v>
@@ -23617,7 +23609,7 @@
         <v>43</v>
       </c>
       <c r="P339" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="Q339" s="1" t="s">
         <v>78</v>
@@ -23696,7 +23688,7 @@
         <v>34</v>
       </c>
       <c r="I341" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J341" s="1" t="s">
         <v>62</v>
@@ -23773,10 +23765,10 @@
         <v>58</v>
       </c>
       <c r="F342" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G342" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H342" s="1" t="s">
         <v>39</v>
@@ -23800,7 +23792,7 @@
         <v>43</v>
       </c>
       <c r="O342" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="P342" s="1" t="s">
         <v>109</v>
@@ -23865,7 +23857,7 @@
         <v>2007.0</v>
       </c>
       <c r="G343" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H343" s="1" t="s">
         <v>90</v>
@@ -23973,7 +23965,7 @@
         <v>58</v>
       </c>
       <c r="F346" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G346" s="5" t="s">
         <v>425</v>
@@ -23982,7 +23974,7 @@
         <v>39</v>
       </c>
       <c r="I346" s="6" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J346" s="1" t="s">
         <v>62</v>
@@ -24000,10 +23992,10 @@
         <v>43</v>
       </c>
       <c r="O346" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="P346" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="Q346" s="1" t="s">
         <v>65</v>
@@ -24081,16 +24073,16 @@
         <v>36</v>
       </c>
       <c r="F349" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G349" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H349" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I349" s="6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J349" s="1" t="s">
         <v>62</v>
@@ -24108,7 +24100,7 @@
         <v>43</v>
       </c>
       <c r="P349" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="Q349" s="1" t="s">
         <v>46</v>
@@ -24181,7 +24173,7 @@
         <v>2012.0</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H351" s="1" t="s">
         <v>39</v>
@@ -24289,7 +24281,7 @@
         <v>67</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H354" s="1" t="s">
         <v>90</v>
@@ -24384,7 +24376,7 @@
         <v>39</v>
       </c>
       <c r="I355" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J355" s="1" t="s">
         <v>62</v>
@@ -24402,7 +24394,7 @@
         <v>43</v>
       </c>
       <c r="O355" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="P355" s="1" t="s">
         <v>258</v>
@@ -24475,7 +24467,7 @@
         <v>2002.0</v>
       </c>
       <c r="G357" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H357" s="1" t="s">
         <v>39</v>
@@ -24730,10 +24722,10 @@
         <v>36</v>
       </c>
       <c r="F369" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="G369" s="5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H369" s="1" t="s">
         <v>90</v>
@@ -24757,7 +24749,7 @@
         <v>43</v>
       </c>
       <c r="P369" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="Q369" s="1" t="s">
         <v>65</v>
@@ -24827,10 +24819,10 @@
         <v>36</v>
       </c>
       <c r="F371" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G371" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="H371" s="1" t="s">
         <v>90</v>
@@ -24927,7 +24919,7 @@
         <v>2019.0</v>
       </c>
       <c r="G373" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H373" s="1" t="s">
         <v>39</v>
@@ -25016,10 +25008,10 @@
         <v>58</v>
       </c>
       <c r="F374" s="5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G374" s="5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H374" s="1" t="s">
         <v>39</v>
@@ -25105,16 +25097,16 @@
         <v>36</v>
       </c>
       <c r="F375" s="5" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G375" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H375" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I375" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="J375" s="1" t="s">
         <v>62</v>
@@ -25213,7 +25205,7 @@
         <v>2017.0</v>
       </c>
       <c r="G378" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H378" s="1" t="s">
         <v>90</v>
@@ -25237,7 +25229,7 @@
         <v>43</v>
       </c>
       <c r="O378" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="P378" s="1" t="s">
         <v>193</v>
@@ -25311,7 +25303,7 @@
         <v>34</v>
       </c>
       <c r="I379" s="6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J379" s="1" t="s">
         <v>62</v>
@@ -25329,7 +25321,7 @@
         <v>43</v>
       </c>
       <c r="P379" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Q379" s="1" t="s">
         <v>46</v>
@@ -25402,7 +25394,7 @@
         <v>1996.0</v>
       </c>
       <c r="G381" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H381" s="1" t="s">
         <v>90</v>
@@ -25596,7 +25588,7 @@
         <v>58</v>
       </c>
       <c r="F385" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G385" s="1">
         <v>2016.0</v>
@@ -25696,10 +25688,10 @@
         <v>36</v>
       </c>
       <c r="F387" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="G387" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H387" s="1" t="s">
         <v>60</v>
@@ -25788,7 +25780,7 @@
         <v>58</v>
       </c>
       <c r="F388" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="G388" s="1" t="s">
         <v>119</v>
@@ -25797,7 +25789,7 @@
         <v>39</v>
       </c>
       <c r="I388" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J388" s="1" t="s">
         <v>62</v>
@@ -25815,10 +25807,10 @@
         <v>158</v>
       </c>
       <c r="O388" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="P388" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="Q388" s="1" t="s">
         <v>46</v>
@@ -25915,7 +25907,7 @@
         <v>92</v>
       </c>
       <c r="P390" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="Q390" s="1" t="s">
         <v>98</v>
@@ -25924,7 +25916,7 @@
         <v>99</v>
       </c>
       <c r="S390" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="T390" s="1" t="s">
         <v>81</v>
@@ -25939,7 +25931,7 @@
         <v>116</v>
       </c>
       <c r="X390" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="Y390" s="1" t="s">
         <v>51</v>
@@ -25999,7 +25991,7 @@
         <v>58</v>
       </c>
       <c r="F393" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="G393" s="1" t="s">
         <v>131</v>
@@ -26088,7 +26080,7 @@
         <v>36</v>
       </c>
       <c r="F394" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="G394" s="1" t="s">
         <v>243</v>
@@ -26180,16 +26172,16 @@
         <v>58</v>
       </c>
       <c r="F395" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="G395" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="H395" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I395" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J395" s="1" t="s">
         <v>62</v>
@@ -26225,7 +26217,7 @@
         <v>116</v>
       </c>
       <c r="X395" s="6" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="Y395" s="1" t="s">
         <v>51</v>
@@ -26363,7 +26355,7 @@
         <v>58</v>
       </c>
       <c r="F398" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="G398" s="1" t="s">
         <v>400</v>
@@ -26477,7 +26469,7 @@
         <v>60</v>
       </c>
       <c r="I401" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J401" s="1" t="s">
         <v>62</v>
@@ -26572,7 +26564,7 @@
         <v>39</v>
       </c>
       <c r="I402" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J402" s="1" t="s">
         <v>41</v>
@@ -26673,7 +26665,7 @@
         <v>58</v>
       </c>
       <c r="F406" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G406" s="1" t="s">
         <v>154</v>
@@ -26765,7 +26757,7 @@
         <v>2014.0</v>
       </c>
       <c r="G407" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H407" s="1" t="s">
         <v>34</v>
@@ -26807,7 +26799,7 @@
         <v>116</v>
       </c>
       <c r="X407" s="6" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="Y407" s="1" t="s">
         <v>49</v>
@@ -26965,7 +26957,7 @@
         <v>1999.0</v>
       </c>
       <c r="G411" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H411" s="1" t="s">
         <v>90</v>
@@ -27175,13 +27167,13 @@
         <v>88</v>
       </c>
       <c r="G417" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H417" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I417" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J417" s="1" t="s">
         <v>62</v>
@@ -27270,7 +27262,7 @@
         <v>39</v>
       </c>
       <c r="I418" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J418" s="1" t="s">
         <v>62</v>
@@ -27366,16 +27358,16 @@
         <v>58</v>
       </c>
       <c r="F421" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G421" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="H421" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I421" s="6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="J421" s="1" t="s">
         <v>62</v>
@@ -27393,7 +27385,7 @@
         <v>181</v>
       </c>
       <c r="O421" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="P421" s="1" t="s">
         <v>87</v>
@@ -27458,16 +27450,16 @@
         <v>58</v>
       </c>
       <c r="F422" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G422" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H422" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I422" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="J422" s="1" t="s">
         <v>62</v>
@@ -27547,10 +27539,10 @@
         <v>36</v>
       </c>
       <c r="F423" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="G423" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H423" s="1" t="s">
         <v>60</v>
@@ -27574,7 +27566,7 @@
         <v>43</v>
       </c>
       <c r="O423" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="P423" s="1" t="s">
         <v>109</v>
@@ -27642,7 +27634,7 @@
         <v>2017.0</v>
       </c>
       <c r="G424" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="H424" s="1" t="s">
         <v>39</v>
@@ -27728,16 +27720,16 @@
         <v>58</v>
       </c>
       <c r="F425" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G425" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="H425" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I425" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J425" s="1" t="s">
         <v>62</v>
@@ -27776,7 +27768,7 @@
         <v>116</v>
       </c>
       <c r="X425" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="Y425" s="1" t="s">
         <v>49</v>
@@ -27823,10 +27815,10 @@
         <v>58</v>
       </c>
       <c r="F426" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G426" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="H426" s="1" t="s">
         <v>39</v>
@@ -27850,7 +27842,7 @@
         <v>43</v>
       </c>
       <c r="O426" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="P426" s="1" t="s">
         <v>77</v>
@@ -27923,10 +27915,10 @@
         <v>58</v>
       </c>
       <c r="F428" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="G428" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H428" s="1" t="s">
         <v>60</v>
@@ -28101,10 +28093,10 @@
         <v>58</v>
       </c>
       <c r="F430" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="G430" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H430" s="1" t="s">
         <v>39</v>
@@ -28190,7 +28182,7 @@
         <v>58</v>
       </c>
       <c r="F431" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G431" s="1" t="s">
         <v>179</v>
@@ -28279,16 +28271,16 @@
         <v>36</v>
       </c>
       <c r="F432" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="G432" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H432" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I432" s="6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J432" s="1" t="s">
         <v>62</v>
@@ -28368,7 +28360,7 @@
         <v>58</v>
       </c>
       <c r="F433" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G433" s="1">
         <v>2018.0</v>
@@ -28377,7 +28369,7 @@
         <v>90</v>
       </c>
       <c r="I433" s="6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="J433" s="1" t="s">
         <v>62</v>
@@ -28395,10 +28387,10 @@
         <v>255</v>
       </c>
       <c r="O433" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="P433" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="Q433" s="1" t="s">
         <v>65</v>
@@ -28419,7 +28411,7 @@
         <v>116</v>
       </c>
       <c r="X433" s="6" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="Y433" s="1" t="s">
         <v>49</v>
@@ -28483,7 +28475,7 @@
         <v>39</v>
       </c>
       <c r="I435" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J435" s="1" t="s">
         <v>62</v>
@@ -28569,7 +28561,7 @@
         <v>58</v>
       </c>
       <c r="F436" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="G436" s="1" t="s">
         <v>38</v>
@@ -28599,7 +28591,7 @@
         <v>44</v>
       </c>
       <c r="P436" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="Q436" s="1" t="s">
         <v>46</v>
@@ -28620,7 +28612,7 @@
         <v>116</v>
       </c>
       <c r="X436" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="Y436" s="1" t="s">
         <v>51</v>
@@ -28699,7 +28691,7 @@
         <v>43</v>
       </c>
       <c r="O438" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="P438" s="1" t="s">
         <v>77</v>
@@ -28772,10 +28764,10 @@
         <v>58</v>
       </c>
       <c r="F440" s="5" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="G440" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H440" s="1" t="s">
         <v>60</v>
@@ -28911,7 +28903,7 @@
         <v>79</v>
       </c>
       <c r="S442" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="T442" s="1" t="s">
         <v>73</v>
@@ -28967,10 +28959,10 @@
         <v>36</v>
       </c>
       <c r="F443" s="5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="G443" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H443" s="1" t="s">
         <v>39</v>
@@ -29059,13 +29051,13 @@
         <v>2018.0</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I444" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J444" s="1" t="s">
         <v>62</v>
@@ -29187,7 +29179,7 @@
         <v>49</v>
       </c>
       <c r="V445" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="W445" s="1" t="s">
         <v>51</v>
@@ -29237,7 +29229,7 @@
         <v>237</v>
       </c>
       <c r="G446" s="5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="H446" s="1" t="s">
         <v>90</v>
@@ -29261,7 +29253,7 @@
         <v>43</v>
       </c>
       <c r="O446" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="P446" s="1" t="s">
         <v>187</v>
@@ -29285,7 +29277,7 @@
         <v>116</v>
       </c>
       <c r="X446" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="Y446" s="1" t="s">
         <v>49</v>
@@ -29332,7 +29324,7 @@
         <v>58</v>
       </c>
       <c r="F447" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G447" s="1" t="s">
         <v>371</v>
@@ -29341,7 +29333,7 @@
         <v>39</v>
       </c>
       <c r="I447" s="6" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J447" s="1" t="s">
         <v>62</v>
@@ -29421,16 +29413,16 @@
         <v>58</v>
       </c>
       <c r="F448" s="5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="G448" s="5" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H448" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I448" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J448" s="1" t="s">
         <v>62</v>
@@ -29448,7 +29440,7 @@
         <v>43</v>
       </c>
       <c r="O448" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="P448" s="1" t="s">
         <v>77</v>
@@ -29516,13 +29508,13 @@
         <v>2012.0</v>
       </c>
       <c r="G449" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="H449" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I449" s="6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J449" s="1" t="s">
         <v>62</v>
@@ -29549,7 +29541,7 @@
         <v>65</v>
       </c>
       <c r="R449" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="S449" s="1" t="s">
         <v>43</v>
@@ -29605,10 +29597,10 @@
         <v>58</v>
       </c>
       <c r="F450" s="5" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G450" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H450" s="1" t="s">
         <v>39</v>
@@ -29699,7 +29691,7 @@
         <v>36</v>
       </c>
       <c r="F452" s="5" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G452" s="1" t="s">
         <v>119</v>
@@ -29831,10 +29823,10 @@
         <v>58</v>
       </c>
       <c r="F458" s="5" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G458" s="5" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H458" s="1" t="s">
         <v>39</v>
@@ -29959,7 +29951,7 @@
         <v>60</v>
       </c>
       <c r="I462" s="6" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="J462" s="1" t="s">
         <v>182</v>
@@ -30055,19 +30047,19 @@
         <v>57</v>
       </c>
       <c r="E465" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F465" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G465" s="5" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="H465" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I465" s="6" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="J465" s="1" t="s">
         <v>62</v>
@@ -30150,13 +30142,13 @@
         <v>225</v>
       </c>
       <c r="G466" s="5" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="H466" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I466" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J466" s="1" t="s">
         <v>41</v>
@@ -30174,7 +30166,7 @@
         <v>43</v>
       </c>
       <c r="P466" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="Q466" s="1" t="s">
         <v>46</v>
@@ -30244,16 +30236,16 @@
         <v>58</v>
       </c>
       <c r="F468" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G468" s="5" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H468" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I468" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J468" s="1" t="s">
         <v>62</v>
@@ -30283,7 +30275,7 @@
         <v>195</v>
       </c>
       <c r="T468" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="U468" s="1" t="s">
         <v>49</v>
@@ -30295,7 +30287,7 @@
         <v>116</v>
       </c>
       <c r="X468" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Y468" s="1" t="s">
         <v>49</v>
@@ -30345,7 +30337,7 @@
         <v>151</v>
       </c>
       <c r="G469" s="5" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="H469" s="1" t="s">
         <v>90</v>
@@ -30369,7 +30361,7 @@
         <v>43</v>
       </c>
       <c r="P469" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="Q469" s="1" t="s">
         <v>65</v>
@@ -30378,7 +30370,7 @@
         <v>43</v>
       </c>
       <c r="S469" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="U469" s="1" t="s">
         <v>104</v>
@@ -30434,7 +30426,7 @@
         <v>144</v>
       </c>
       <c r="G470" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H470" s="1" t="s">
         <v>39</v>
@@ -30520,10 +30512,10 @@
         <v>58</v>
       </c>
       <c r="F471" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G471" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H471" s="1" t="s">
         <v>39</v>
@@ -30571,7 +30563,7 @@
         <v>116</v>
       </c>
       <c r="X471" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Y471" s="1" t="s">
         <v>51</v>
@@ -30618,13 +30610,13 @@
         <v>205</v>
       </c>
       <c r="G472" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H472" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I472" s="6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J472" s="1" t="s">
         <v>62</v>
@@ -30642,7 +30634,7 @@
         <v>43</v>
       </c>
       <c r="O472" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="P472" s="1" t="s">
         <v>77</v>
@@ -30731,10 +30723,10 @@
         <v>58</v>
       </c>
       <c r="F476" s="5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G476" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H476" s="1" t="s">
         <v>39</v>
@@ -30823,7 +30815,7 @@
         <v>58</v>
       </c>
       <c r="F477" s="5" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G477" s="1" t="s">
         <v>145</v>
@@ -30949,10 +30941,10 @@
         <v>58</v>
       </c>
       <c r="F483" s="5" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G483" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H483" s="1" t="s">
         <v>39</v>
@@ -31143,10 +31135,10 @@
         <v>36</v>
       </c>
       <c r="F487" s="5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G487" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H487" s="1" t="s">
         <v>60</v>
@@ -31243,7 +31235,7 @@
         <v>2018.0</v>
       </c>
       <c r="G489" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H489" s="1" t="s">
         <v>34</v>
@@ -31270,7 +31262,7 @@
         <v>116</v>
       </c>
       <c r="P489" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="Q489" s="1" t="s">
         <v>46</v>
@@ -31332,13 +31324,13 @@
         <v>486</v>
       </c>
       <c r="G490" s="5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="H490" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I490" s="6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="J490" s="1" t="s">
         <v>62</v>
@@ -31380,7 +31372,7 @@
         <v>116</v>
       </c>
       <c r="X490" s="6" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="Y490" s="1" t="s">
         <v>49</v>
@@ -31404,7 +31396,7 @@
         <v>54</v>
       </c>
       <c r="AF490" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AG490" s="1" t="s">
         <v>56</v>
@@ -31430,13 +31422,13 @@
         <v>2015.0</v>
       </c>
       <c r="G491" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="H491" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I491" s="6" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="J491" s="1" t="s">
         <v>41</v>
@@ -31521,10 +31513,10 @@
         <v>58</v>
       </c>
       <c r="F493" s="5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="G493" s="5" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="H493" s="1" t="s">
         <v>90</v>
@@ -31713,7 +31705,7 @@
         <v>58</v>
       </c>
       <c r="F496" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G496" s="1" t="s">
         <v>358</v>
@@ -31740,7 +31732,7 @@
         <v>43</v>
       </c>
       <c r="O496" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="P496" s="1" t="s">
         <v>87</v>
@@ -31999,16 +31991,16 @@
         <v>58</v>
       </c>
       <c r="F501" s="5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G501" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="H501" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I501" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J501" s="1" t="s">
         <v>62</v>
@@ -32091,16 +32083,16 @@
         <v>58</v>
       </c>
       <c r="F502" s="5" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G502" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="H502" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I502" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J502" s="1" t="s">
         <v>62</v>
@@ -32689,7 +32681,7 @@
         <v>-1.0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="3">
@@ -32697,7 +32689,7 @@
         <v>-2.0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="4">
@@ -32705,7 +32697,7 @@
         <v>-3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6">
@@ -32718,7 +32710,7 @@
         <v>-1.0</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="8">
@@ -32726,7 +32718,7 @@
         <v>-2.0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="9">
@@ -32734,12 +32726,12 @@
         <v>-3.0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="12">
@@ -32762,7 +32754,7 @@
         <v>91</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="16">
@@ -32770,7 +32762,7 @@
         <v>305</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="17">
@@ -32778,7 +32770,7 @@
         <v>433</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="18">
@@ -32786,7 +32778,7 @@
         <v>120</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="19">
@@ -32794,7 +32786,7 @@
         <v>464</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="20">
@@ -32802,7 +32794,7 @@
         <v>450</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="21">
@@ -32827,7 +32819,7 @@
     </row>
     <row r="25">
       <c r="B25" s="10" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="26">
@@ -32842,7 +32834,7 @@
     </row>
     <row r="29">
       <c r="A29" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>